<commit_message>
Updated to take Data Sheet name dynamically for the test case
</commit_message>
<xml_diff>
--- a/Test Case/eApp Test Data.xlsx
+++ b/Test Case/eApp Test Data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssahoo43\D_Drive\eAppBHFAutomation\Test Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D5D88C-FF44-4810-8CB6-DBBB91F2EA32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9865D419-B2A8-4FE4-A507-50DCE68E5D06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12756" windowHeight="2868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
-    <sheet name="TestData" sheetId="4" r:id="rId2"/>
-    <sheet name="ListValues" sheetId="3" r:id="rId3"/>
+    <sheet name="FRA" sheetId="4" r:id="rId2"/>
+    <sheet name="FA" sheetId="5" r:id="rId3"/>
+    <sheet name="ListValues" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestData!$A$2:$H$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FRA!$A$2:$G$103</definedName>
     <definedName name="P_Country">ListValues!$D$2:$D$24</definedName>
     <definedName name="P_Frequency">ListValues!$G$2:$G$5</definedName>
     <definedName name="P_Gender">ListValues!$E$2:$E$3</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="348">
   <si>
     <t>SLNo</t>
   </si>
@@ -1077,6 +1078,18 @@
   </si>
   <si>
     <t>Variable Prime Options - NY</t>
+  </si>
+  <si>
+    <t>TestData Sheet</t>
+  </si>
+  <si>
+    <t>Variable Prime Options</t>
+  </si>
+  <si>
+    <t>FRA</t>
+  </si>
+  <si>
+    <t>FA</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1214,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1245,7 +1258,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1595,19 +1607,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1615,10 +1629,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1626,10 +1643,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1637,10 +1657,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1648,10 +1671,13 @@
         <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1659,10 +1685,13 @@
         <v>131</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1670,12 +1699,15 @@
         <v>242</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>347</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>P_Yes_No</formula1>
     </dataValidation>
   </dataValidations>
@@ -1687,26 +1719,25 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52F2985-23B5-4103-BDA8-163FD22005C0}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H200"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.44140625" style="22" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.44140625" style="21" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="35.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="35.33203125" style="9" customWidth="1"/>
     <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1724,11 +1755,8 @@
       <c r="G1" s="3">
         <v>4</v>
       </c>
-      <c r="H1" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1750,15 +1778,12 @@
       <c r="G2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>241</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1774,11 +1799,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>241</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>331</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1797,11 +1822,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>238</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -1818,11 +1843,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>238</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>239</v>
       </c>
       <c r="C6" t="s">
@@ -1842,11 +1867,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>238</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>239</v>
       </c>
       <c r="C7" t="s">
@@ -1865,11 +1890,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>238</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>239</v>
       </c>
       <c r="C8" t="s">
@@ -1886,11 +1911,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>123</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1901,13 +1926,12 @@
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>342</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1919,20 +1943,16 @@
       <c r="E10" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="9" t="str">
-        <f>UPPER(C10)</f>
-        <v>SELECTPLAN</v>
-      </c>
+      <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>123</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1943,13 +1963,12 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1965,13 +1984,12 @@
       <c r="G12" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1984,13 +2002,12 @@
       <c r="G13" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>136</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -2004,13 +2021,12 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>129</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -2021,13 +2037,12 @@
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
         <v>136</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -2041,13 +2056,12 @@
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>195</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -2061,13 +2075,12 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="21" t="s">
         <v>136</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -2081,13 +2094,12 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>137</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -2101,13 +2113,12 @@
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>138</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -2121,13 +2132,12 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>139</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -2141,13 +2151,12 @@
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="21" t="s">
         <v>124</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -2161,13 +2170,12 @@
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="21" t="s">
         <v>140</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -2181,13 +2189,12 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="21" t="s">
         <v>141</v>
       </c>
       <c r="C24" s="9" t="s">
@@ -2201,13 +2208,12 @@
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="21" t="s">
         <v>247</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -2221,13 +2227,12 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -2239,13 +2244,12 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -2259,13 +2263,12 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="18"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C28" s="9" t="s">
@@ -2275,14 +2278,13 @@
         <v>120</v>
       </c>
       <c r="F28" s="9"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G28" s="23"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>146</v>
       </c>
       <c r="C29" s="9" t="s">
@@ -2295,14 +2297,13 @@
         <v>120</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G29" s="23"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="21" t="s">
         <v>145</v>
       </c>
       <c r="C30" s="9" t="s">
@@ -2312,14 +2313,13 @@
         <v>120</v>
       </c>
       <c r="F30" s="9"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G30" s="23"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="21" t="s">
         <v>148</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -2332,14 +2332,13 @@
         <v>120</v>
       </c>
       <c r="F31" s="9"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G31" s="23"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>146</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -2353,13 +2352,12 @@
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>147</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -2373,13 +2371,12 @@
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="21" t="s">
         <v>148</v>
       </c>
       <c r="C34" s="9" t="s">
@@ -2393,13 +2390,12 @@
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="10"/>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -2413,13 +2409,12 @@
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="21" t="s">
         <v>149</v>
       </c>
       <c r="C36" s="9" t="s">
@@ -2433,13 +2428,12 @@
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="21" t="s">
         <v>150</v>
       </c>
       <c r="C37" s="9" t="s">
@@ -2453,13 +2447,12 @@
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="21" t="s">
         <v>151</v>
       </c>
       <c r="C38" s="9" t="s">
@@ -2470,13 +2463,12 @@
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>152</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -2487,13 +2479,12 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="21" t="s">
         <v>153</v>
       </c>
       <c r="C40" s="9" t="s">
@@ -2507,13 +2498,12 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="21" t="s">
         <v>154</v>
       </c>
       <c r="C41" s="9" t="s">
@@ -2527,13 +2517,12 @@
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="21" t="s">
         <v>155</v>
       </c>
       <c r="C42" s="9" t="s">
@@ -2547,19 +2536,18 @@
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="19" t="s">
         <v>108</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -2567,13 +2555,12 @@
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="21" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="9" t="s">
@@ -2587,13 +2574,12 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="21" t="s">
         <v>156</v>
       </c>
       <c r="C45" s="9" t="s">
@@ -2607,19 +2593,18 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="14"/>
-      <c r="H45" s="9"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="21" t="s">
         <v>157</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="19" t="s">
         <v>169</v>
       </c>
       <c r="E46" s="9" t="s">
@@ -2627,19 +2612,18 @@
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="14"/>
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="21" t="s">
         <v>158</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="19" t="s">
         <v>170</v>
       </c>
       <c r="E47" s="9" t="s">
@@ -2647,19 +2631,18 @@
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="14"/>
-      <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="21" t="s">
         <v>159</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="D48" s="20" t="s">
         <v>245</v>
       </c>
       <c r="E48" s="9" t="s">
@@ -2667,19 +2650,18 @@
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="14"/>
-      <c r="H48" s="9"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="21" t="s">
         <v>160</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="D49" s="19" t="s">
         <v>108</v>
       </c>
       <c r="E49" s="9" t="s">
@@ -2687,19 +2669,18 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="14"/>
-      <c r="H49" s="9"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="21" t="s">
         <v>161</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="19" t="s">
         <v>108</v>
       </c>
       <c r="E50" s="9" t="s">
@@ -2707,403 +2688,382 @@
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="14"/>
-      <c r="H50" s="9"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="20"/>
+      <c r="D51" s="19"/>
       <c r="E51" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="14"/>
-      <c r="H51" s="9"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D52" s="20" t="s">
+      <c r="D52" s="19" t="s">
         <v>252</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F52" s="9"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="9"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G52" s="23"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D53" s="20"/>
+      <c r="D53" s="19"/>
       <c r="E53" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F53" s="9"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="9"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G53" s="23"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B54" s="22" t="s">
+      <c r="B54" s="21" t="s">
         <v>146</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D54" s="20" t="s">
+      <c r="D54" s="19" t="s">
         <v>253</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F54" s="9"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="9"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G54" s="23"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="21" t="s">
         <v>251</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="20"/>
+      <c r="D55" s="19"/>
       <c r="E55" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F55" s="9"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="9"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G55" s="23"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="21" t="s">
         <v>146</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="D56" s="19" t="s">
         <v>253</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F56" s="9"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="9"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G56" s="23"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="21" t="s">
         <v>254</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="20" t="s">
+      <c r="D57" s="19" t="s">
         <v>259</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F57" s="9"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="9"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G57" s="23"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="21" t="s">
         <v>255</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="19" t="s">
         <v>260</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F58" s="9"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="9"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G58" s="23"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="21" t="s">
         <v>256</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D59" s="19" t="s">
         <v>261</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F59" s="9"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="9"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G59" s="23"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="21" t="s">
         <v>149</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D60" s="20"/>
+      <c r="D60" s="19"/>
       <c r="E60" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F60" s="9"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="9"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G60" s="23"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="21" t="s">
         <v>257</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="19" t="s">
         <v>262</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F61" s="9"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="9"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G61" s="23"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="21" t="s">
         <v>151</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D62" s="20" t="s">
+      <c r="D62" s="19" t="s">
         <v>263</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F62" s="9"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="9"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G62" s="23"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="21" t="s">
         <v>152</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D63" s="20"/>
+      <c r="D63" s="19"/>
       <c r="E63" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F63" s="9"/>
-      <c r="G63" s="24"/>
-      <c r="H63" s="9"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G63" s="23"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="21" t="s">
         <v>153</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D64" s="20" t="s">
+      <c r="D64" s="19" t="s">
         <v>264</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F64" s="9"/>
-      <c r="G64" s="24"/>
-      <c r="H64" s="9"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G64" s="23"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="21" t="s">
         <v>154</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D65" s="20" t="s">
+      <c r="D65" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F65" s="9"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="9"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G65" s="23"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B66" s="22" t="s">
+      <c r="B66" s="21" t="s">
         <v>258</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D66" s="29">
+      <c r="D66" s="28">
         <v>63103</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F66" s="9"/>
-      <c r="G66" s="24"/>
-      <c r="H66" s="9"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G66" s="23"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D67" s="20" t="s">
+      <c r="D67" s="19" t="s">
         <v>108</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F67" s="9"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="9"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G67" s="23"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="B68" s="21" t="s">
         <v>265</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D68" s="20" t="s">
+      <c r="D68" s="19" t="s">
         <v>267</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F68" s="9"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="9"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G68" s="23"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="21" t="s">
         <v>158</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D69" s="20" t="s">
+      <c r="D69" s="19" t="s">
         <v>268</v>
       </c>
       <c r="E69" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F69" s="9"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="9"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G69" s="23"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="21" t="s">
         <v>159</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D70" s="21" t="s">
+      <c r="D70" s="20" t="s">
         <v>266</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F70" s="9"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="9"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G70" s="23"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="21" t="s">
         <v>269</v>
       </c>
       <c r="C71" s="9" t="s">
@@ -3116,14 +3076,13 @@
         <v>120</v>
       </c>
       <c r="F71" s="9"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="9"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G71" s="23"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="21" t="s">
         <v>270</v>
       </c>
       <c r="C72" s="9" t="s">
@@ -3136,14 +3095,13 @@
         <v>120</v>
       </c>
       <c r="F72" s="9"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="9"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G72" s="23"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="21" t="s">
         <v>271</v>
       </c>
       <c r="C73" s="9" t="s">
@@ -3153,14 +3111,13 @@
         <v>120</v>
       </c>
       <c r="F73" s="9"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="9"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G73" s="23"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="21" t="s">
         <v>272</v>
       </c>
       <c r="C74" s="9" t="s">
@@ -3173,14 +3130,13 @@
         <v>120</v>
       </c>
       <c r="F74" s="9"/>
-      <c r="G74" s="24"/>
-      <c r="H74" s="9"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G74" s="23"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B75" s="22" t="s">
+      <c r="B75" s="21" t="s">
         <v>273</v>
       </c>
       <c r="C75" s="9" t="s">
@@ -3190,14 +3146,13 @@
         <v>120</v>
       </c>
       <c r="F75" s="9"/>
-      <c r="G75" s="24"/>
-      <c r="H75" s="9"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G75" s="23"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B76" s="22" t="s">
+      <c r="B76" s="21" t="s">
         <v>274</v>
       </c>
       <c r="C76" s="9" t="s">
@@ -3210,14 +3165,13 @@
         <v>120</v>
       </c>
       <c r="F76" s="9"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G76" s="23"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="21" t="s">
         <v>247</v>
       </c>
       <c r="C77" s="9" t="s">
@@ -3230,14 +3184,13 @@
         <v>120</v>
       </c>
       <c r="F77" s="9"/>
-      <c r="G77" s="24"/>
-      <c r="H77" s="9"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G77" s="23"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B78" s="22" t="s">
+      <c r="B78" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C78" s="9" t="s">
@@ -3247,14 +3200,13 @@
         <v>120</v>
       </c>
       <c r="F78" s="9"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="9"/>
-    </row>
-    <row r="79" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G78" s="23"/>
+    </row>
+    <row r="79" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C79" s="15" t="s">
@@ -3267,13 +3219,12 @@
         <v>120</v>
       </c>
       <c r="F79" s="9"/>
-      <c r="H79" s="15"/>
-    </row>
-    <row r="80" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B80" s="22" t="s">
+      <c r="B80" s="21" t="s">
         <v>179</v>
       </c>
       <c r="C80" s="9" t="s">
@@ -3286,13 +3237,12 @@
         <v>120</v>
       </c>
       <c r="F80" s="9"/>
-      <c r="H80" s="15"/>
-    </row>
-    <row r="81" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B81" s="22" t="s">
+      <c r="B81" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C81" s="9" t="s">
@@ -3303,51 +3253,48 @@
         <v>120</v>
       </c>
       <c r="F81" s="9"/>
-      <c r="H81" s="15"/>
-    </row>
-    <row r="82" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:7" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B82" s="22" t="s">
+      <c r="B82" s="21" t="s">
         <v>156</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D82" s="25" t="s">
+      <c r="D82" s="24" t="s">
         <v>278</v>
       </c>
       <c r="E82" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F82" s="9"/>
-      <c r="H82" s="15"/>
-    </row>
-    <row r="83" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:7" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B83" s="22" t="s">
+      <c r="B83" s="21" t="s">
         <v>280</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D83" s="25" t="s">
+      <c r="D83" s="24" t="s">
         <v>279</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F83" s="9"/>
-      <c r="H83" s="15"/>
-    </row>
-    <row r="84" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="B84" s="22" t="s">
+      <c r="B84" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C84" s="9" t="s">
@@ -3358,13 +3305,12 @@
         <v>120</v>
       </c>
       <c r="F84" s="9"/>
-      <c r="H84" s="15"/>
-    </row>
-    <row r="85" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="21" t="s">
         <v>146</v>
       </c>
       <c r="C85" s="9" t="s">
@@ -3377,32 +3323,30 @@
         <v>120</v>
       </c>
       <c r="F85" s="9"/>
-      <c r="H85" s="15"/>
-    </row>
-    <row r="86" spans="1:8" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:7" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B86" s="22" t="s">
+      <c r="B86" s="21" t="s">
         <v>281</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D86" s="25" t="s">
+      <c r="D86" s="24" t="s">
         <v>283</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F86" s="9"/>
-      <c r="H86" s="15"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="22" t="s">
+      <c r="B87" s="21" t="s">
         <v>173</v>
       </c>
       <c r="C87" s="9" t="s">
@@ -3416,13 +3360,12 @@
       </c>
       <c r="F87" s="9"/>
       <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B88" s="22" t="s">
+      <c r="B88" s="21" t="s">
         <v>174</v>
       </c>
       <c r="C88" s="9" t="s">
@@ -3435,13 +3378,12 @@
         <v>120</v>
       </c>
       <c r="F88" s="9"/>
-      <c r="H88" s="9"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B89" s="22" t="s">
+      <c r="B89" s="21" t="s">
         <v>175</v>
       </c>
       <c r="C89" s="9" t="s">
@@ -3455,11 +3397,11 @@
       </c>
       <c r="F89" s="9"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B90" s="22" t="s">
+      <c r="B90" s="21" t="s">
         <v>146</v>
       </c>
       <c r="C90" s="9" t="s">
@@ -3472,13 +3414,12 @@
         <v>120</v>
       </c>
       <c r="F90" s="9"/>
-      <c r="H90" s="9"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B91" s="22" t="s">
+      <c r="B91" s="21" t="s">
         <v>147</v>
       </c>
       <c r="C91" s="9" t="s">
@@ -3491,13 +3432,12 @@
         <v>120</v>
       </c>
       <c r="F91" s="9"/>
-      <c r="H91" s="9"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B92" s="22" t="s">
+      <c r="B92" s="21" t="s">
         <v>148</v>
       </c>
       <c r="C92" s="9" t="s">
@@ -3510,13 +3450,12 @@
         <v>120</v>
       </c>
       <c r="F92" s="9"/>
-      <c r="H92" s="9"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B93" s="22" t="s">
+      <c r="B93" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C93" s="9" t="s">
@@ -3529,13 +3468,12 @@
         <v>120</v>
       </c>
       <c r="F93" s="9"/>
-      <c r="H93" s="9"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B94" s="22" t="s">
+      <c r="B94" s="21" t="s">
         <v>176</v>
       </c>
       <c r="C94" s="9" t="s">
@@ -3548,13 +3486,12 @@
         <v>120</v>
       </c>
       <c r="F94" s="9"/>
-      <c r="H94" s="9"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B95" s="22" t="s">
+      <c r="B95" s="21" t="s">
         <v>156</v>
       </c>
       <c r="C95" s="9" t="s">
@@ -3567,51 +3504,48 @@
         <v>120</v>
       </c>
       <c r="F95" s="9"/>
-      <c r="H95" s="9"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B96" s="22" t="s">
+      <c r="B96" s="21" t="s">
         <v>157</v>
       </c>
       <c r="C96" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D96" s="20" t="s">
+      <c r="D96" s="19" t="s">
         <v>169</v>
       </c>
       <c r="E96" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F96" s="9"/>
-      <c r="H96" s="9"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B97" s="22" t="s">
+      <c r="B97" s="21" t="s">
         <v>158</v>
       </c>
       <c r="C97" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D97" s="20" t="s">
+      <c r="D97" s="19" t="s">
         <v>170</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F97" s="9"/>
-      <c r="H97" s="9"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B98" s="22" t="s">
+      <c r="B98" s="21" t="s">
         <v>149</v>
       </c>
       <c r="C98" s="9" t="s">
@@ -3625,13 +3559,12 @@
       </c>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
-      <c r="H98" s="9"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="21" t="s">
         <v>150</v>
       </c>
       <c r="C99" s="9" t="s">
@@ -3645,13 +3578,12 @@
       </c>
       <c r="F99" s="9"/>
       <c r="G99" s="17"/>
-      <c r="H99" s="19"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B100" s="22" t="s">
+      <c r="B100" s="21" t="s">
         <v>151</v>
       </c>
       <c r="C100" s="9" t="s">
@@ -3665,11 +3597,11 @@
       </c>
       <c r="F100" s="9"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B101" s="22" t="s">
+      <c r="B101" s="21" t="s">
         <v>152</v>
       </c>
       <c r="C101" s="9" t="s">
@@ -3682,13 +3614,12 @@
         <v>120</v>
       </c>
       <c r="F101" s="9"/>
-      <c r="H101" s="9"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B102" s="22" t="s">
+      <c r="B102" s="21" t="s">
         <v>154</v>
       </c>
       <c r="C102" s="9" t="s">
@@ -3701,13 +3632,12 @@
         <v>120</v>
       </c>
       <c r="F102" s="9"/>
-      <c r="H102" s="9"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B103" s="22" t="s">
+      <c r="B103" s="21" t="s">
         <v>155</v>
       </c>
       <c r="C103" s="9" t="s">
@@ -3720,19 +3650,18 @@
         <v>120</v>
       </c>
       <c r="F103" s="9"/>
-      <c r="H103" s="9"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B104" s="22" t="s">
+      <c r="B104" s="21" t="s">
         <v>177</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D104" s="20" t="s">
+      <c r="D104" s="19" t="s">
         <v>108</v>
       </c>
       <c r="E104" s="9" t="s">
@@ -3740,11 +3669,11 @@
       </c>
       <c r="F104" s="9"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B105" s="22" t="s">
+      <c r="B105" s="21" t="s">
         <v>178</v>
       </c>
       <c r="C105" s="9" t="s">
@@ -3758,11 +3687,11 @@
       </c>
       <c r="F105" s="9"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B106" s="22" t="s">
+      <c r="B106" s="21" t="s">
         <v>211</v>
       </c>
       <c r="C106" s="9" t="s">
@@ -3776,11 +3705,11 @@
       </c>
       <c r="F106" s="9"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B107" s="22" t="s">
+      <c r="B107" s="21" t="s">
         <v>284</v>
       </c>
       <c r="C107" s="9" t="s">
@@ -3793,13 +3722,12 @@
         <v>120</v>
       </c>
       <c r="F107" s="9"/>
-      <c r="H107" s="9"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B108" s="22" t="s">
+      <c r="B108" s="21" t="s">
         <v>285</v>
       </c>
       <c r="C108" s="9" t="s">
@@ -3813,11 +3741,11 @@
       </c>
       <c r="F108" s="9"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B109" s="22" t="s">
+      <c r="B109" s="21" t="s">
         <v>286</v>
       </c>
       <c r="C109" s="9" t="s">
@@ -3830,13 +3758,12 @@
         <v>120</v>
       </c>
       <c r="F109" s="9"/>
-      <c r="H109" s="9"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B110" s="22" t="s">
+      <c r="B110" s="21" t="s">
         <v>289</v>
       </c>
       <c r="C110" s="9" t="s">
@@ -3849,89 +3776,84 @@
         <v>120</v>
       </c>
       <c r="F110" s="9"/>
-      <c r="H110" s="9"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B111" s="22" t="s">
+      <c r="B111" s="21" t="s">
         <v>290</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D111" s="20" t="s">
+      <c r="D111" s="19" t="s">
         <v>291</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F111" s="9"/>
-      <c r="H111" s="9"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B112" s="22" t="s">
+      <c r="B112" s="21" t="s">
         <v>294</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D112" s="20" t="s">
+      <c r="D112" s="19" t="s">
         <v>292</v>
       </c>
       <c r="E112" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F112" s="9"/>
-      <c r="H112" s="9"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B113" s="22" t="s">
+      <c r="B113" s="21" t="s">
         <v>295</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D113" s="24"/>
+      <c r="D113" s="23"/>
       <c r="E113" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F113" s="9"/>
       <c r="G113" s="9"/>
-      <c r="H113" s="9"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B114" s="22" t="s">
+      <c r="B114" s="21" t="s">
         <v>296</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D114" s="24" t="s">
+      <c r="D114" s="23" t="s">
         <v>293</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F114" s="9"/>
-      <c r="G114" s="24"/>
-      <c r="H114" s="24"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G114" s="23"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B115" s="22" t="s">
+      <c r="B115" s="21" t="s">
         <v>297</v>
       </c>
       <c r="C115" s="9" t="s">
@@ -3945,11 +3867,11 @@
       </c>
       <c r="F115" s="9"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B116" s="22" t="s">
+      <c r="B116" s="21" t="s">
         <v>298</v>
       </c>
       <c r="C116" s="9" t="s">
@@ -3959,13 +3881,12 @@
         <v>120</v>
       </c>
       <c r="F116" s="9"/>
-      <c r="H116" s="9"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B117" s="22" t="s">
+      <c r="B117" s="21" t="s">
         <v>299</v>
       </c>
       <c r="C117" s="9" t="s">
@@ -3978,13 +3899,12 @@
         <v>120</v>
       </c>
       <c r="F117" s="9"/>
-      <c r="H117" s="9"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B118" s="22" t="s">
+      <c r="B118" s="21" t="s">
         <v>300</v>
       </c>
       <c r="C118" s="9" t="s">
@@ -3997,19 +3917,18 @@
         <v>120</v>
       </c>
       <c r="F118" s="9"/>
-      <c r="H118" s="9"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B119" s="22" t="s">
+      <c r="B119" s="21" t="s">
         <v>301</v>
       </c>
       <c r="C119" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D119" s="20" t="s">
+      <c r="D119" s="19" t="s">
         <v>108</v>
       </c>
       <c r="E119" s="9" t="s">
@@ -4017,11 +3936,11 @@
       </c>
       <c r="F119" s="9"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B120" s="22" t="s">
+      <c r="B120" s="21" t="s">
         <v>302</v>
       </c>
       <c r="C120" s="9" t="s">
@@ -4035,11 +3954,11 @@
       </c>
       <c r="F120" s="9"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B121" s="22" t="s">
+      <c r="B121" s="21" t="s">
         <v>304</v>
       </c>
       <c r="C121" s="9" t="s">
@@ -4053,11 +3972,11 @@
       </c>
       <c r="F121" s="9"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B122" s="22" t="s">
+      <c r="B122" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C122" s="9" t="s">
@@ -4068,7 +3987,7 @@
       </c>
       <c r="F122" s="9"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>234</v>
       </c>
@@ -4086,7 +4005,7 @@
       </c>
       <c r="F123" s="9"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>234</v>
       </c>
@@ -4104,11 +4023,11 @@
       </c>
       <c r="F124" s="9"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>186</v>
       </c>
-      <c r="B125" s="22" t="s">
+      <c r="B125" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C125" s="9" t="s">
@@ -4122,11 +4041,11 @@
       </c>
       <c r="F125" s="9"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>186</v>
       </c>
-      <c r="B126" s="22" t="s">
+      <c r="B126" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C126" s="9" t="s">
@@ -4137,17 +4056,17 @@
       </c>
       <c r="F126" s="9"/>
     </row>
-    <row r="127" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>186</v>
       </c>
-      <c r="B127" s="22" t="s">
+      <c r="B127" s="21" t="s">
         <v>196</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D127" s="25" t="s">
+      <c r="D127" s="24" t="s">
         <v>305</v>
       </c>
       <c r="E127" s="9" t="s">
@@ -4155,17 +4074,17 @@
       </c>
       <c r="F127" s="9"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>248</v>
       </c>
-      <c r="B128" s="22" t="s">
+      <c r="B128" s="21" t="s">
         <v>186</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D128" s="25"/>
+      <c r="D128" s="24"/>
       <c r="E128" s="9" t="s">
         <v>120</v>
       </c>
@@ -4175,13 +4094,13 @@
       <c r="A129" t="s">
         <v>186</v>
       </c>
-      <c r="B129" s="22" t="s">
+      <c r="B129" s="21" t="s">
         <v>196</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D129" s="25" t="s">
+      <c r="D129" s="24" t="s">
         <v>305</v>
       </c>
       <c r="E129" s="9" t="s">
@@ -4193,7 +4112,7 @@
       <c r="A130" t="s">
         <v>186</v>
       </c>
-      <c r="B130" s="22" t="s">
+      <c r="B130" s="21" t="s">
         <v>196</v>
       </c>
       <c r="C130" s="9" t="s">
@@ -4211,7 +4130,7 @@
       <c r="A131" t="s">
         <v>186</v>
       </c>
-      <c r="B131" s="22" t="s">
+      <c r="B131" s="21" t="s">
         <v>185</v>
       </c>
       <c r="C131" s="9" t="s">
@@ -4229,7 +4148,7 @@
       <c r="A132" t="s">
         <v>186</v>
       </c>
-      <c r="B132" s="22" t="s">
+      <c r="B132" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C132" s="9" t="s">
@@ -4244,7 +4163,7 @@
       <c r="A133" t="s">
         <v>187</v>
       </c>
-      <c r="B133" s="22" t="s">
+      <c r="B133" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C133" s="9" t="s">
@@ -4262,7 +4181,7 @@
       <c r="A134" t="s">
         <v>187</v>
       </c>
-      <c r="B134" s="22" t="s">
+      <c r="B134" s="21" t="s">
         <v>188</v>
       </c>
       <c r="C134" s="9" t="s">
@@ -4280,7 +4199,7 @@
       <c r="A135" t="s">
         <v>187</v>
       </c>
-      <c r="B135" s="22" t="s">
+      <c r="B135" s="21" t="s">
         <v>197</v>
       </c>
       <c r="C135" s="9" t="s">
@@ -4298,7 +4217,7 @@
       <c r="A136" t="s">
         <v>187</v>
       </c>
-      <c r="B136" s="22" t="s">
+      <c r="B136" s="21" t="s">
         <v>198</v>
       </c>
       <c r="C136" s="9" t="s">
@@ -4316,7 +4235,7 @@
       <c r="A137" t="s">
         <v>187</v>
       </c>
-      <c r="B137" s="22" t="s">
+      <c r="B137" s="21" t="s">
         <v>188</v>
       </c>
       <c r="C137" s="9" t="s">
@@ -4331,7 +4250,7 @@
       <c r="A138" t="s">
         <v>187</v>
       </c>
-      <c r="B138" s="22" t="s">
+      <c r="B138" s="21" t="s">
         <v>188</v>
       </c>
       <c r="C138" s="9" t="s">
@@ -4364,7 +4283,7 @@
       <c r="A140" t="s">
         <v>187</v>
       </c>
-      <c r="B140" s="22" t="s">
+      <c r="B140" s="21" t="s">
         <v>188</v>
       </c>
       <c r="C140" s="9" t="s">
@@ -4382,7 +4301,7 @@
       <c r="A141" t="s">
         <v>187</v>
       </c>
-      <c r="B141" s="22" t="s">
+      <c r="B141" s="21" t="s">
         <v>188</v>
       </c>
       <c r="C141" s="9" t="s">
@@ -4400,7 +4319,7 @@
       <c r="A142" t="s">
         <v>187</v>
       </c>
-      <c r="B142" s="22" t="s">
+      <c r="B142" s="21" t="s">
         <v>189</v>
       </c>
       <c r="C142" s="9" t="s">
@@ -4418,13 +4337,13 @@
       <c r="A143" t="s">
         <v>187</v>
       </c>
-      <c r="B143" s="22" t="s">
+      <c r="B143" s="21" t="s">
         <v>190</v>
       </c>
       <c r="C143" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D143" s="23">
+      <c r="D143" s="22">
         <v>40397</v>
       </c>
       <c r="E143" s="9" t="s">
@@ -4436,7 +4355,7 @@
       <c r="A144" t="s">
         <v>187</v>
       </c>
-      <c r="B144" s="22" t="s">
+      <c r="B144" s="21" t="s">
         <v>124</v>
       </c>
       <c r="C144" s="9" t="s">
@@ -4454,7 +4373,7 @@
       <c r="A145" t="s">
         <v>187</v>
       </c>
-      <c r="B145" s="22" t="s">
+      <c r="B145" s="21" t="s">
         <v>191</v>
       </c>
       <c r="C145" s="9" t="s">
@@ -4472,7 +4391,7 @@
       <c r="A146" t="s">
         <v>187</v>
       </c>
-      <c r="B146" s="22" t="s">
+      <c r="B146" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C146" s="9" t="s">
@@ -4487,13 +4406,13 @@
       <c r="A147" t="s">
         <v>200</v>
       </c>
-      <c r="B147" s="22" t="s">
+      <c r="B147" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C147" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D147" s="22" t="s">
+      <c r="D147" s="21" t="s">
         <v>232</v>
       </c>
       <c r="E147" s="9" t="s">
@@ -4505,13 +4424,13 @@
       <c r="A148" t="s">
         <v>200</v>
       </c>
-      <c r="B148" s="22" t="s">
+      <c r="B148" s="21" t="s">
         <v>199</v>
       </c>
       <c r="C148" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D148" s="22" t="s">
+      <c r="D148" s="21" t="s">
         <v>29</v>
       </c>
       <c r="E148" s="9" t="s">
@@ -4523,13 +4442,13 @@
       <c r="A149" t="s">
         <v>200</v>
       </c>
-      <c r="B149" s="22" t="s">
+      <c r="B149" s="21" t="s">
         <v>199</v>
       </c>
       <c r="C149" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D149" s="22" t="s">
+      <c r="D149" s="21" t="s">
         <v>5</v>
       </c>
       <c r="E149" s="9" t="s">
@@ -4541,13 +4460,13 @@
       <c r="A150" t="s">
         <v>200</v>
       </c>
-      <c r="B150" s="22" t="s">
+      <c r="B150" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C150" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D150" s="22"/>
+      <c r="D150" s="21"/>
       <c r="E150" s="9" t="s">
         <v>120</v>
       </c>
@@ -4557,16 +4476,16 @@
       <c r="A151" t="s">
         <v>215</v>
       </c>
-      <c r="B151" s="22" t="s">
+      <c r="B151" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C151" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D151" s="22" t="s">
+      <c r="D151" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="E151" s="22" t="s">
+      <c r="E151" s="21" t="s">
         <v>233</v>
       </c>
       <c r="F151" s="9"/>
@@ -4575,30 +4494,30 @@
       <c r="A152" t="s">
         <v>215</v>
       </c>
-      <c r="B152" s="22" t="s">
+      <c r="B152" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C152" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D152" s="22"/>
-      <c r="E152" s="22"/>
+      <c r="D152" s="21"/>
+      <c r="E152" s="21"/>
       <c r="F152" s="9"/>
     </row>
     <row r="153" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>215</v>
       </c>
-      <c r="B153" s="22" t="s">
+      <c r="B153" s="21" t="s">
         <v>204</v>
       </c>
       <c r="C153" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D153" s="22" t="s">
+      <c r="D153" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="E153" s="22" t="s">
+      <c r="E153" s="21" t="s">
         <v>307</v>
       </c>
       <c r="F153" s="9"/>
@@ -4607,16 +4526,16 @@
       <c r="A154" t="s">
         <v>215</v>
       </c>
-      <c r="B154" s="22" t="s">
+      <c r="B154" s="21" t="s">
         <v>209</v>
       </c>
       <c r="C154" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D154" s="22" t="s">
+      <c r="D154" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="E154" s="22" t="s">
+      <c r="E154" s="21" t="s">
         <v>308</v>
       </c>
       <c r="F154" s="9"/>
@@ -4625,30 +4544,30 @@
       <c r="A155" t="s">
         <v>248</v>
       </c>
-      <c r="B155" s="22" t="s">
+      <c r="B155" s="21" t="s">
         <v>215</v>
       </c>
       <c r="C155" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D155" s="22"/>
-      <c r="E155" s="22"/>
+      <c r="D155" s="21"/>
+      <c r="E155" s="21"/>
       <c r="F155" s="9"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>215</v>
       </c>
-      <c r="B156" s="22" t="s">
+      <c r="B156" s="21" t="s">
         <v>211</v>
       </c>
       <c r="C156" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D156" s="22" t="s">
+      <c r="D156" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="E156" s="22" t="s">
+      <c r="E156" s="21" t="s">
         <v>309</v>
       </c>
       <c r="F156" s="9"/>
@@ -4657,16 +4576,16 @@
       <c r="A157" t="s">
         <v>215</v>
       </c>
-      <c r="B157" s="22" t="s">
+      <c r="B157" s="21" t="s">
         <v>201</v>
       </c>
       <c r="C157" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D157" s="22" t="s">
+      <c r="D157" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E157" s="22" t="s">
+      <c r="E157" s="21" t="s">
         <v>29</v>
       </c>
       <c r="F157" s="9"/>
@@ -4675,16 +4594,16 @@
       <c r="A158" t="s">
         <v>215</v>
       </c>
-      <c r="B158" s="22" t="s">
+      <c r="B158" s="21" t="s">
         <v>202</v>
       </c>
       <c r="C158" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D158" s="22" t="s">
+      <c r="D158" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E158" s="22" t="s">
+      <c r="E158" s="21" t="s">
         <v>29</v>
       </c>
       <c r="F158" s="9"/>
@@ -4693,7 +4612,7 @@
       <c r="A159" t="s">
         <v>215</v>
       </c>
-      <c r="B159" s="22" t="s">
+      <c r="B159" s="21" t="s">
         <v>203</v>
       </c>
       <c r="C159" s="9" t="s">
@@ -4711,7 +4630,7 @@
       <c r="A160" t="s">
         <v>215</v>
       </c>
-      <c r="B160" s="22" t="s">
+      <c r="B160" s="21" t="s">
         <v>175</v>
       </c>
       <c r="C160" s="9" t="s">
@@ -4729,7 +4648,7 @@
       <c r="A161" t="s">
         <v>215</v>
       </c>
-      <c r="B161" s="22" t="s">
+      <c r="B161" s="21" t="s">
         <v>204</v>
       </c>
       <c r="C161" s="9" t="s">
@@ -4747,7 +4666,7 @@
       <c r="A162" t="s">
         <v>215</v>
       </c>
-      <c r="B162" s="22" t="s">
+      <c r="B162" s="21" t="s">
         <v>147</v>
       </c>
       <c r="C162" s="9" t="s">
@@ -4765,7 +4684,7 @@
       <c r="A163" t="s">
         <v>215</v>
       </c>
-      <c r="B163" s="22" t="s">
+      <c r="B163" s="21" t="s">
         <v>205</v>
       </c>
       <c r="C163" s="9" t="s">
@@ -4783,7 +4702,7 @@
       <c r="A164" t="s">
         <v>215</v>
       </c>
-      <c r="B164" s="22" t="s">
+      <c r="B164" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C164" s="9" t="s">
@@ -4795,16 +4714,16 @@
       <c r="A165" t="s">
         <v>215</v>
       </c>
-      <c r="B165" s="22" t="s">
+      <c r="B165" s="21" t="s">
         <v>157</v>
       </c>
       <c r="C165" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D165" s="20" t="s">
+      <c r="D165" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="E165" s="20" t="s">
+      <c r="E165" s="19" t="s">
         <v>313</v>
       </c>
       <c r="F165" s="9"/>
@@ -4813,16 +4732,16 @@
       <c r="A166" t="s">
         <v>215</v>
       </c>
-      <c r="B166" s="22" t="s">
+      <c r="B166" s="21" t="s">
         <v>137</v>
       </c>
       <c r="C166" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D166" s="29">
+      <c r="D166" s="28">
         <v>435243</v>
       </c>
-      <c r="E166" s="20" t="s">
+      <c r="E166" s="19" t="s">
         <v>335</v>
       </c>
       <c r="F166" s="9"/>
@@ -4831,7 +4750,7 @@
       <c r="A167" t="s">
         <v>215</v>
       </c>
-      <c r="B167" s="22" t="s">
+      <c r="B167" s="21" t="s">
         <v>206</v>
       </c>
       <c r="C167" s="9" t="s">
@@ -4849,16 +4768,16 @@
       <c r="A168" t="s">
         <v>215</v>
       </c>
-      <c r="B168" s="22" t="s">
+      <c r="B168" s="21" t="s">
         <v>207</v>
       </c>
       <c r="C168" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D168" s="20" t="s">
+      <c r="D168" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="E168" s="20" t="s">
+      <c r="E168" s="19" t="s">
         <v>315</v>
       </c>
       <c r="F168" s="9"/>
@@ -4867,7 +4786,7 @@
       <c r="A169" t="s">
         <v>215</v>
       </c>
-      <c r="B169" s="22" t="s">
+      <c r="B169" s="21" t="s">
         <v>208</v>
       </c>
       <c r="C169" s="9" t="s">
@@ -4885,16 +4804,16 @@
       <c r="A170" t="s">
         <v>215</v>
       </c>
-      <c r="B170" s="22" t="s">
+      <c r="B170" s="21" t="s">
         <v>209</v>
       </c>
       <c r="C170" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D170" s="20">
+      <c r="D170" s="19">
         <v>100</v>
       </c>
-      <c r="E170" s="20">
+      <c r="E170" s="19">
         <v>100</v>
       </c>
       <c r="F170" s="9"/>
@@ -4903,7 +4822,7 @@
       <c r="A171" t="s">
         <v>215</v>
       </c>
-      <c r="B171" s="22" t="s">
+      <c r="B171" s="21" t="s">
         <v>210</v>
       </c>
       <c r="C171" s="9" t="s">
@@ -4921,7 +4840,7 @@
       <c r="A172" t="s">
         <v>215</v>
       </c>
-      <c r="B172" s="22" t="s">
+      <c r="B172" s="21" t="s">
         <v>211</v>
       </c>
       <c r="C172" s="9" t="s">
@@ -4939,7 +4858,7 @@
       <c r="A173" t="s">
         <v>215</v>
       </c>
-      <c r="B173" s="22" t="s">
+      <c r="B173" s="21" t="s">
         <v>212</v>
       </c>
       <c r="C173" s="9" t="s">
@@ -4957,7 +4876,7 @@
       <c r="A174" t="s">
         <v>215</v>
       </c>
-      <c r="B174" s="22" t="s">
+      <c r="B174" s="21" t="s">
         <v>213</v>
       </c>
       <c r="C174" s="9" t="s">
@@ -4975,16 +4894,16 @@
       <c r="A175" t="s">
         <v>215</v>
       </c>
-      <c r="B175" s="22" t="s">
+      <c r="B175" s="21" t="s">
         <v>214</v>
       </c>
       <c r="C175" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D175" s="30">
+      <c r="D175" s="29">
         <v>12500</v>
       </c>
-      <c r="E175" s="26" t="s">
+      <c r="E175" s="25" t="s">
         <v>330</v>
       </c>
       <c r="F175" s="9"/>
@@ -4993,7 +4912,7 @@
       <c r="A176" t="s">
         <v>215</v>
       </c>
-      <c r="B176" s="22" t="s">
+      <c r="B176" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C176" s="9" t="s">
@@ -5005,7 +4924,7 @@
       <c r="A177" t="s">
         <v>230</v>
       </c>
-      <c r="B177" s="22" t="s">
+      <c r="B177" s="21" t="s">
         <v>317</v>
       </c>
       <c r="C177" s="9" t="s">
@@ -5017,7 +4936,7 @@
       <c r="A178" t="s">
         <v>230</v>
       </c>
-      <c r="B178" s="22" t="s">
+      <c r="B178" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C178" s="9" t="s">
@@ -5029,7 +4948,7 @@
       <c r="A179" t="s">
         <v>227</v>
       </c>
-      <c r="B179" s="22" t="s">
+      <c r="B179" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C179" s="9" t="s">
@@ -5047,7 +4966,7 @@
       <c r="A180" t="s">
         <v>227</v>
       </c>
-      <c r="B180" s="22" t="s">
+      <c r="B180" s="21" t="s">
         <v>218</v>
       </c>
       <c r="C180" s="9" t="s">
@@ -5065,7 +4984,7 @@
       <c r="A181" t="s">
         <v>227</v>
       </c>
-      <c r="B181" s="22" t="s">
+      <c r="B181" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C181" s="9" t="s">
@@ -5077,16 +4996,16 @@
       <c r="A182" t="s">
         <v>227</v>
       </c>
-      <c r="B182" s="22" t="s">
+      <c r="B182" s="21" t="s">
         <v>219</v>
       </c>
       <c r="C182" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D182" s="25" t="s">
+      <c r="D182" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="E182" s="25" t="s">
+      <c r="E182" s="24" t="s">
         <v>318</v>
       </c>
       <c r="F182" s="9"/>
@@ -5119,7 +5038,7 @@
       <c r="A185" t="s">
         <v>230</v>
       </c>
-      <c r="B185" s="22" t="s">
+      <c r="B185" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C185" s="9" t="s">
@@ -5131,16 +5050,16 @@
       <c r="A186" t="s">
         <v>227</v>
       </c>
-      <c r="B186" s="22" t="s">
+      <c r="B186" s="21" t="s">
         <v>221</v>
       </c>
       <c r="C186" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D186" s="25" t="s">
+      <c r="D186" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="E186" s="25" t="s">
+      <c r="E186" s="24" t="s">
         <v>320</v>
       </c>
       <c r="F186" s="9"/>
@@ -5149,7 +5068,7 @@
       <c r="A187" t="s">
         <v>227</v>
       </c>
-      <c r="B187" s="22" t="s">
+      <c r="B187" s="21" t="s">
         <v>219</v>
       </c>
       <c r="C187" s="9" t="s">
@@ -5167,7 +5086,7 @@
       <c r="A188" t="s">
         <v>227</v>
       </c>
-      <c r="B188" s="22" t="s">
+      <c r="B188" s="21" t="s">
         <v>220</v>
       </c>
       <c r="C188" s="9" t="s">
@@ -5185,7 +5104,7 @@
       <c r="A189" t="s">
         <v>227</v>
       </c>
-      <c r="B189" s="22" t="s">
+      <c r="B189" s="21" t="s">
         <v>221</v>
       </c>
       <c r="C189" s="9" t="s">
@@ -5203,7 +5122,7 @@
       <c r="A190" t="s">
         <v>227</v>
       </c>
-      <c r="B190" s="22" t="s">
+      <c r="B190" s="21" t="s">
         <v>222</v>
       </c>
       <c r="C190" s="9" t="s">
@@ -5221,7 +5140,7 @@
       <c r="A191" t="s">
         <v>227</v>
       </c>
-      <c r="B191" s="22" t="s">
+      <c r="B191" s="21" t="s">
         <v>223</v>
       </c>
       <c r="C191" s="9" t="s">
@@ -5239,7 +5158,7 @@
       <c r="A192" t="s">
         <v>227</v>
       </c>
-      <c r="B192" s="22" t="s">
+      <c r="B192" s="21" t="s">
         <v>224</v>
       </c>
       <c r="C192" s="9" t="s">
@@ -5257,7 +5176,7 @@
       <c r="A193" t="s">
         <v>227</v>
       </c>
-      <c r="B193" s="22" t="s">
+      <c r="B193" s="21" t="s">
         <v>225</v>
       </c>
       <c r="C193" s="9" t="s">
@@ -5275,16 +5194,16 @@
       <c r="A194" t="s">
         <v>227</v>
       </c>
-      <c r="B194" s="22" t="s">
+      <c r="B194" s="21" t="s">
         <v>226</v>
       </c>
       <c r="C194" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D194" s="23">
+      <c r="D194" s="22">
         <v>43690</v>
       </c>
-      <c r="E194" s="23">
+      <c r="E194" s="22">
         <v>43690</v>
       </c>
       <c r="F194" s="9"/>
@@ -5293,7 +5212,7 @@
       <c r="A195" t="s">
         <v>227</v>
       </c>
-      <c r="B195" s="22" t="s">
+      <c r="B195" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C195" s="9" t="s">
@@ -5305,7 +5224,7 @@
       <c r="A196" t="s">
         <v>229</v>
       </c>
-      <c r="B196" s="22" t="s">
+      <c r="B196" s="21" t="s">
         <v>135</v>
       </c>
       <c r="C196" s="9" t="s">
@@ -5323,7 +5242,7 @@
       <c r="A197" t="s">
         <v>229</v>
       </c>
-      <c r="B197" s="22" t="s">
+      <c r="B197" s="21" t="s">
         <v>228</v>
       </c>
       <c r="C197" s="9" t="s">
@@ -5341,10 +5260,10 @@
       <c r="C198" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D198" s="25" t="s">
+      <c r="D198" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="E198" s="25" t="s">
+      <c r="E198" s="24" t="s">
         <v>325</v>
       </c>
       <c r="F198" s="9"/>
@@ -5353,16 +5272,16 @@
       <c r="A199" t="s">
         <v>234</v>
       </c>
-      <c r="B199" s="22" t="s">
+      <c r="B199" s="21" t="s">
         <v>235</v>
       </c>
       <c r="C199" t="s">
         <v>119</v>
       </c>
-      <c r="D199" s="28" t="s">
+      <c r="D199" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="E199" s="27" t="s">
+      <c r="E199" s="26" t="s">
         <v>336</v>
       </c>
       <c r="F199" s="9"/>
@@ -5371,7 +5290,7 @@
       <c r="A200" t="s">
         <v>234</v>
       </c>
-      <c r="B200" s="22" t="s">
+      <c r="B200" s="21" t="s">
         <v>236</v>
       </c>
       <c r="C200" t="s">
@@ -5380,12 +5299,12 @@
       <c r="F200" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H103" xr:uid="{08FCDD39-550A-416F-A1E8-17A8732FCA8E}"/>
+  <autoFilter ref="A2:G103" xr:uid="{08FCDD39-550A-416F-A1E8-17A8732FCA8E}"/>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G36" xr:uid="{63BF2A67-F2B3-4C32-A201-03503A960558}">
       <formula1>P_Frequency</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G98:H98 G35 G113:H113" xr:uid="{94FFB3B2-D830-4E80-8C74-1F62E2705CEC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G98 G35 G113" xr:uid="{94FFB3B2-D830-4E80-8C74-1F62E2705CEC}">
       <formula1>P_UWClass</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G87 G32" xr:uid="{9E71B626-1F3E-4FB0-8918-E2EBF903A19C}">
@@ -5411,6 +5330,108 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740F98E4-4E45-4FFC-9391-45E7D275E888}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.44140625" style="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{A1BBD2C2-525F-4852-980E-12513D31FCBE}">
+      <formula1>Step</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I52"/>

</xml_diff>

<commit_message>
Updated test data and created data for Trunk
</commit_message>
<xml_diff>
--- a/Test Case/eApp Test Data.xlsx
+++ b/Test Case/eApp Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssahoo43\D_Drive\eAppBHFAutomation\Test Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05C75B5-C684-4897-BB8E-782898E85EFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A83740E-CFBC-4A1C-BA22-0A300E2CABBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12756" windowHeight="2868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12756" windowHeight="2868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
@@ -2180,7 +2180,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -2363,7 +2363,7 @@
   <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -11998,8 +11998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09FF1B8-A6E4-4273-AAE7-8B972A5FB15D}">
   <dimension ref="A1:F231"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15702,7 +15702,7 @@
         <v>118</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>231</v>
+        <v>5</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>